<commit_message>
new design implement and some functionality changes
</commit_message>
<xml_diff>
--- a/public/sample-file/sample.xlsx
+++ b/public/sample-file/sample.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -31,13 +31,26 @@
     <t xml:space="preserve">amount</t>
   </si>
   <si>
+    <t xml:space="preserve">date</t>
+  </si>
+  <si>
     <t xml:space="preserve">00060856</t>
   </si>
   <si>
+    <t xml:space="preserve">01 mar 2023, 06:09 pm
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">b</t>
   </si>
   <si>
+    <t xml:space="preserve">08 mar 2023, 02:19 am</t>
+  </si>
+  <si>
     <t xml:space="preserve">c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 mar 2023, 12:00 pm</t>
   </si>
 </sst>
 </file>
@@ -112,13 +125,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -138,13 +155,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="270" zoomScaleNormal="270" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -156,16 +173,22 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="24.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>120</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -173,10 +196,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>20</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -184,10 +210,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>30</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
download match,unmatch and ignore record
</commit_message>
<xml_diff>
--- a/public/sample-file/sample.xlsx
+++ b/public/sample-file/sample.xlsx
@@ -37,8 +37,7 @@
     <t xml:space="preserve">00060856</t>
   </si>
   <si>
-    <t xml:space="preserve">01 mar 2023, 06:09 pm
-</t>
+    <t xml:space="preserve">09 mar 2023, 02:19 am</t>
   </si>
   <si>
     <t xml:space="preserve">b</t>
@@ -47,7 +46,7 @@
     <t xml:space="preserve">08 mar 2023, 02:19 am</t>
   </si>
   <si>
-    <t xml:space="preserve">c</t>
+    <t xml:space="preserve">00006511</t>
   </si>
   <si>
     <t xml:space="preserve">10 mar 2023, 12:00 pm</t>
@@ -158,10 +157,13 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="270" zoomScaleNormal="270" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.97"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -173,11 +175,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="24.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
@@ -185,7 +187,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>120</v>
+        <v>1200</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>5</v>
@@ -201,7 +203,7 @@
       <c r="C3" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -213,9 +215,9 @@
         <v>8</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="D4" s="0" t="s">
+        <v>10000000</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>